<commit_message>
Added new quests for the raid, new quest items and even NPCs
</commit_message>
<xml_diff>
--- a/resources/data-imports/Monsters/delusional-memories-raid-monsters.xlsx
+++ b/resources/data-imports/Monsters/delusional-memories-raid-monsters.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="84">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -188,6 +188,9 @@
   </si>
   <si>
     <t xml:space="preserve">14600587432-19931660316</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mothers Sleep</t>
   </si>
   <si>
     <t xml:space="preserve">Judge of Emotion</t>
@@ -360,16 +363,20 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -567,2112 +574,2118 @@
   </sheetPr>
   <dimension ref="A1:AX15"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AS2" activeCellId="0" sqref="AS2:AS15"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AI1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AN3" activeCellId="0" sqref="AN3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="5.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="36.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="3" style="0" width="13.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="20.73"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="10.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="18.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="13.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="21.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="11.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="16.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="10.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="11.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="13.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="6.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="12.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="13.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="25" style="0" width="25.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="27" style="0" width="18.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="0" width="20.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="0" width="15.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="31" style="0" width="18.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="32" style="0" width="19.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="33" style="0" width="24.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="34" style="0" width="27.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="35" style="0" width="15.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="36" min="36" style="0" width="19.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="37" min="37" style="0" width="16.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="38" min="38" style="0" width="20.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="39" min="39" style="0" width="33.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="40" min="40" style="0" width="24.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="41" min="41" style="0" width="21.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="43" min="42" style="0" width="16.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="44" min="44" style="0" width="15.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="46" min="45" style="0" width="17.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="47" min="47" style="0" width="14.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="49" min="48" style="0" width="26.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="50" min="50" style="0" width="24.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="5.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="36.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="3" style="1" width="13.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="20.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="10.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="18.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="13.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="21.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="11.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="16.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="10.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="1" width="11.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="1" width="13.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="1" width="6.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="1" width="12.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="1" width="13.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="25" style="1" width="25.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="27" style="1" width="18.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="1" width="20.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="1" width="15.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="31" style="1" width="18.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="32" style="1" width="19.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="33" style="1" width="24.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="34" style="1" width="27.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="35" style="1" width="15.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="36" min="36" style="1" width="19.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="37" min="37" style="1" width="16.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="38" min="38" style="1" width="20.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="39" min="39" style="1" width="33.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="40" min="40" style="1" width="24.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="41" min="41" style="1" width="21.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="43" min="42" style="1" width="16.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="44" min="44" style="1" width="15.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="46" min="45" style="1" width="17.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="47" min="47" style="1" width="14.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="49" min="48" style="1" width="26.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="50" min="50" style="1" width="24.71"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="O1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="P1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="Q1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="R1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="S1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="T1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="U1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="V1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="W1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="X1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Y1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="Z1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AA1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AB1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AC1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AD1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AE1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AF1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AG1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AH1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="AI1" s="1" t="s">
+      <c r="AI1" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="AJ1" s="1" t="s">
+      <c r="AJ1" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="AK1" s="1" t="s">
+      <c r="AK1" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="AL1" s="1" t="s">
+      <c r="AL1" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="AM1" s="1" t="s">
+      <c r="AM1" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="AN1" s="1" t="s">
+      <c r="AN1" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="AO1" s="1" t="s">
+      <c r="AO1" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AP1" s="1" t="s">
+      <c r="AP1" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="AQ1" s="1" t="s">
+      <c r="AQ1" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="AR1" s="1" t="s">
+      <c r="AR1" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="AS1" s="1" t="s">
+      <c r="AS1" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="AT1" s="1" t="s">
+      <c r="AT1" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="AU1" s="1" t="s">
+      <c r="AU1" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="AV1" s="1" t="s">
+      <c r="AV1" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="AW1" s="1" t="s">
+      <c r="AW1" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="AX1" s="1" t="s">
+      <c r="AX1" s="2" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
+      <c r="A2" s="1" t="n">
         <v>518</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C2" s="2" t="n">
+      <c r="C2" s="3" t="n">
         <v>87200339685.342</v>
       </c>
-      <c r="D2" s="2" t="n">
+      <c r="D2" s="3" t="n">
         <v>87200339685.342</v>
       </c>
-      <c r="E2" s="2" t="n">
+      <c r="E2" s="3" t="n">
         <v>87200339685.342</v>
       </c>
-      <c r="F2" s="2" t="n">
+      <c r="F2" s="3" t="n">
         <v>87200339685.342</v>
       </c>
-      <c r="G2" s="2" t="n">
+      <c r="G2" s="3" t="n">
         <v>87200339685.342</v>
       </c>
-      <c r="H2" s="2" t="n">
+      <c r="H2" s="3" t="n">
         <v>87200339685.342</v>
       </c>
-      <c r="I2" s="2" t="n">
+      <c r="I2" s="3" t="n">
         <v>87200339685.342</v>
       </c>
-      <c r="J2" s="2" t="n">
+      <c r="J2" s="3" t="n">
         <v>87200339685.342</v>
       </c>
-      <c r="K2" s="0" t="n">
+      <c r="K2" s="1" t="n">
         <v>0.62369236762792</v>
       </c>
-      <c r="L2" s="0" t="n">
+      <c r="L2" s="1" t="n">
         <v>0.62369236762792</v>
       </c>
-      <c r="M2" s="0" t="n">
+      <c r="M2" s="1" t="n">
         <v>0.62369236762792</v>
       </c>
-      <c r="N2" s="0" t="n">
+      <c r="N2" s="1" t="n">
         <v>0.62369236762792</v>
       </c>
-      <c r="P2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="R2" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="S2" s="0" t="n">
+      <c r="P2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="R2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="S2" s="1" t="n">
         <v>5001</v>
       </c>
-      <c r="T2" s="0" t="s">
+      <c r="T2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="U2" s="2" t="n">
+      <c r="U2" s="3" t="n">
         <v>108.504718979316</v>
       </c>
-      <c r="V2" s="0" t="n">
+      <c r="V2" s="1" t="n">
         <v>0.177493181726</v>
       </c>
-      <c r="W2" s="0" t="n">
+      <c r="W2" s="1" t="n">
         <v>6425925873.481</v>
       </c>
-      <c r="X2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y2" s="0" t="s">
+      <c r="X2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y2" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="Z2" s="0" t="s">
+      <c r="Z2" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="AA2" s="2" t="n">
+      <c r="AA2" s="3" t="n">
         <v>87200339685.342</v>
       </c>
-      <c r="AB2" s="2" t="n">
+      <c r="AB2" s="3" t="n">
         <v>87200339685.342</v>
       </c>
-      <c r="AC2" s="0" t="n">
+      <c r="AC2" s="1" t="n">
         <v>0.62369236762792</v>
       </c>
-      <c r="AD2" s="0" t="n">
+      <c r="AD2" s="1" t="n">
         <v>0.62369236762792</v>
       </c>
-      <c r="AE2" s="0" t="n">
+      <c r="AE2" s="1" t="n">
         <v>0.62369236762792</v>
       </c>
-      <c r="AF2" s="0" t="n">
+      <c r="AF2" s="1" t="n">
         <v>0.62369236762792</v>
       </c>
-      <c r="AG2" s="0" t="n">
+      <c r="AG2" s="1" t="n">
         <v>0.363362739242865</v>
       </c>
-      <c r="AH2" s="0" t="n">
+      <c r="AH2" s="1" t="n">
         <v>0.363362739242865</v>
       </c>
-      <c r="AI2" s="0" t="n">
+      <c r="AI2" s="1" t="n">
         <v>0.373183551323945</v>
       </c>
-      <c r="AJ2" s="0" t="n">
+      <c r="AJ2" s="1" t="n">
         <v>0.373183551323945</v>
       </c>
-      <c r="AK2" s="0" t="n">
+      <c r="AK2" s="1" t="n">
         <v>0.373183551323945</v>
       </c>
-      <c r="AL2" s="0" t="n">
+      <c r="AL2" s="1" t="n">
         <v>0.373183551323945</v>
       </c>
-      <c r="AM2" s="0" t="s">
+      <c r="AM2" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="AN2" s="0" t="n">
+      <c r="AN2" s="1" t="n">
         <v>0.05</v>
       </c>
-      <c r="AO2" s="0" t="s">
+      <c r="AO2" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="AQ2" s="0" t="n">
+      <c r="AQ2" s="1" t="n">
         <v>0.14969332667883</v>
       </c>
-      <c r="AR2" s="0" t="n">
+      <c r="AR2" s="1" t="n">
         <v>0.0945436433326112</v>
       </c>
-      <c r="AS2" s="0" t="n">
+      <c r="AS2" s="1" t="n">
         <v>0.0721814916756006</v>
       </c>
-      <c r="AT2" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="AV2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AW2" s="0" t="n">
+      <c r="AT2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AV2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW2" s="1" t="n">
         <v>0.283178388283094</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
+      <c r="A3" s="1" t="n">
         <v>519</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="C3" s="2" t="n">
+      <c r="C3" s="3" t="n">
         <v>92199796760.5217</v>
       </c>
-      <c r="D3" s="2" t="n">
+      <c r="D3" s="3" t="n">
         <v>92199796760.5217</v>
       </c>
-      <c r="E3" s="2" t="n">
+      <c r="E3" s="3" t="n">
         <v>92199796760.5217</v>
       </c>
-      <c r="F3" s="2" t="n">
+      <c r="F3" s="3" t="n">
         <v>92199796760.5217</v>
       </c>
-      <c r="G3" s="2" t="n">
+      <c r="G3" s="3" t="n">
         <v>92199796760.5217</v>
       </c>
-      <c r="H3" s="2" t="n">
+      <c r="H3" s="3" t="n">
         <v>92199796760.5217</v>
       </c>
-      <c r="I3" s="2" t="n">
+      <c r="I3" s="3" t="n">
         <v>92199796760.5217</v>
       </c>
-      <c r="J3" s="2" t="n">
+      <c r="J3" s="3" t="n">
         <v>92199796760.5217</v>
       </c>
-      <c r="K3" s="0" t="n">
+      <c r="K3" s="1" t="n">
         <v>0.646757758767536</v>
       </c>
-      <c r="L3" s="0" t="n">
+      <c r="L3" s="1" t="n">
         <v>0.646757758767536</v>
       </c>
-      <c r="M3" s="0" t="n">
+      <c r="M3" s="1" t="n">
         <v>0.646757758767536</v>
       </c>
-      <c r="N3" s="0" t="n">
+      <c r="N3" s="1" t="n">
         <v>0.646757758767536</v>
       </c>
-      <c r="P3" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q3" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="R3" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="S3" s="0" t="n">
+      <c r="P3" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="R3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="S3" s="1" t="n">
         <v>5001</v>
       </c>
-      <c r="T3" s="0" t="s">
+      <c r="T3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="U3" s="2" t="n">
+      <c r="U3" s="3" t="n">
         <v>124.814779420242</v>
       </c>
-      <c r="V3" s="0" t="n">
+      <c r="V3" s="1" t="n">
         <v>0.199851997828024</v>
       </c>
-      <c r="W3" s="0" t="n">
+      <c r="W3" s="1" t="n">
         <v>8144671479.8239</v>
       </c>
-      <c r="X3" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y3" s="0" t="s">
+      <c r="X3" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y3" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="Z3" s="0" t="s">
+      <c r="Z3" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="AA3" s="2" t="n">
+      <c r="AA3" s="3" t="n">
         <v>92199796760.5217</v>
       </c>
-      <c r="AB3" s="2" t="n">
+      <c r="AB3" s="3" t="n">
         <v>92199796760.5217</v>
       </c>
-      <c r="AC3" s="0" t="n">
+      <c r="AC3" s="1" t="n">
         <v>0.646757758767536</v>
       </c>
-      <c r="AD3" s="0" t="n">
+      <c r="AD3" s="1" t="n">
         <v>0.646757758767536</v>
       </c>
-      <c r="AE3" s="0" t="n">
+      <c r="AE3" s="1" t="n">
         <v>0.646757758767536</v>
       </c>
-      <c r="AF3" s="0" t="n">
+      <c r="AF3" s="1" t="n">
         <v>0.646757758767536</v>
       </c>
-      <c r="AG3" s="0" t="n">
+      <c r="AG3" s="1" t="n">
         <v>0.387200221542281</v>
       </c>
-      <c r="AH3" s="0" t="n">
+      <c r="AH3" s="1" t="n">
         <v>0.387200221542281</v>
       </c>
-      <c r="AI3" s="0" t="n">
+      <c r="AI3" s="1" t="n">
         <v>0.39685035208295</v>
       </c>
-      <c r="AJ3" s="0" t="n">
+      <c r="AJ3" s="1" t="n">
         <v>0.39685035208295</v>
       </c>
-      <c r="AK3" s="0" t="n">
+      <c r="AK3" s="1" t="n">
         <v>0.39685035208295</v>
       </c>
-      <c r="AL3" s="0" t="n">
+      <c r="AL3" s="1" t="n">
         <v>0.39685035208295</v>
       </c>
-      <c r="AO3" s="0" t="s">
+      <c r="AM3" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AN3" s="1" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="AO3" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="AQ3" s="0" t="n">
+      <c r="AQ3" s="1" t="n">
         <v>0.167191054480982</v>
       </c>
-      <c r="AR3" s="0" t="n">
+      <c r="AR3" s="1" t="n">
         <v>0.102778791750184</v>
       </c>
-      <c r="AS3" s="0" t="n">
+      <c r="AS3" s="1" t="n">
         <v>0.0791704573889415</v>
       </c>
-      <c r="AT3" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="AV3" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AW3" s="0" t="n">
+      <c r="AT3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AV3" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW3" s="1" t="n">
         <v>0.307598729682108</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="n">
+      <c r="A4" s="1" t="n">
         <v>520</v>
       </c>
-      <c r="B4" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="C4" s="2" t="n">
+      <c r="B4" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C4" s="3" t="n">
         <v>97485887708.1927</v>
       </c>
-      <c r="D4" s="2" t="n">
+      <c r="D4" s="3" t="n">
         <v>97485887708.1927</v>
       </c>
-      <c r="E4" s="2" t="n">
+      <c r="E4" s="3" t="n">
         <v>97485887708.1927</v>
       </c>
-      <c r="F4" s="2" t="n">
+      <c r="F4" s="3" t="n">
         <v>97485887708.1927</v>
       </c>
-      <c r="G4" s="2" t="n">
+      <c r="G4" s="3" t="n">
         <v>97485887708.1927</v>
       </c>
-      <c r="H4" s="2" t="n">
+      <c r="H4" s="3" t="n">
         <v>97485887708.1927</v>
       </c>
-      <c r="I4" s="2" t="n">
+      <c r="I4" s="3" t="n">
         <v>97485887708.1927</v>
       </c>
-      <c r="J4" s="2" t="n">
+      <c r="J4" s="3" t="n">
         <v>97485887708.1927</v>
       </c>
-      <c r="K4" s="0" t="n">
+      <c r="K4" s="1" t="n">
         <v>0.670676154202277</v>
       </c>
-      <c r="L4" s="0" t="n">
+      <c r="L4" s="1" t="n">
         <v>0.670676154202277</v>
       </c>
-      <c r="M4" s="0" t="n">
+      <c r="M4" s="1" t="n">
         <v>0.670676154202277</v>
       </c>
-      <c r="N4" s="0" t="n">
+      <c r="N4" s="1" t="n">
         <v>0.670676154202277</v>
       </c>
-      <c r="P4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="R4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="S4" s="0" t="n">
+      <c r="P4" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="R4" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="S4" s="1" t="n">
         <v>5001</v>
       </c>
-      <c r="T4" s="0" t="s">
+      <c r="T4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="U4" s="2" t="n">
+      <c r="U4" s="3" t="n">
         <v>143.576512692443</v>
       </c>
-      <c r="V4" s="0" t="n">
+      <c r="V4" s="1" t="n">
         <v>0.22502735399442</v>
       </c>
-      <c r="W4" s="0" t="n">
+      <c r="W4" s="1" t="n">
         <v>10323130832.8681</v>
       </c>
-      <c r="X4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y4" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="Z4" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="AA4" s="2" t="n">
+      <c r="X4" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y4" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="Z4" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="AA4" s="3" t="n">
         <v>97485887708.1927</v>
       </c>
-      <c r="AB4" s="2" t="n">
+      <c r="AB4" s="3" t="n">
         <v>97485887708.1927</v>
       </c>
-      <c r="AC4" s="0" t="n">
+      <c r="AC4" s="1" t="n">
         <v>0.670676154202277</v>
       </c>
-      <c r="AD4" s="0" t="n">
+      <c r="AD4" s="1" t="n">
         <v>0.670676154202277</v>
       </c>
-      <c r="AE4" s="0" t="n">
+      <c r="AE4" s="1" t="n">
         <v>0.670676154202277</v>
       </c>
-      <c r="AF4" s="0" t="n">
+      <c r="AF4" s="1" t="n">
         <v>0.670676154202277</v>
       </c>
-      <c r="AG4" s="0" t="n">
+      <c r="AG4" s="1" t="n">
         <v>0.412601500843995</v>
       </c>
-      <c r="AH4" s="0" t="n">
+      <c r="AH4" s="1" t="n">
         <v>0.412601500843995</v>
       </c>
-      <c r="AI4" s="0" t="n">
+      <c r="AI4" s="1" t="n">
         <v>0.422018069632579</v>
       </c>
-      <c r="AJ4" s="0" t="n">
+      <c r="AJ4" s="1" t="n">
         <v>0.422018069632579</v>
       </c>
-      <c r="AK4" s="0" t="n">
+      <c r="AK4" s="1" t="n">
         <v>0.422018069632579</v>
       </c>
-      <c r="AL4" s="0" t="n">
+      <c r="AL4" s="1" t="n">
         <v>0.422018069632579</v>
       </c>
-      <c r="AM4" s="0" t="s">
-        <v>58</v>
-      </c>
-      <c r="AN4" s="0" t="n">
+      <c r="AM4" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AN4" s="1" t="n">
         <v>0.07</v>
       </c>
-      <c r="AO4" s="0" t="s">
+      <c r="AO4" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="AQ4" s="0" t="n">
+      <c r="AQ4" s="1" t="n">
         <v>0.186734100434791</v>
       </c>
-      <c r="AR4" s="0" t="n">
+      <c r="AR4" s="1" t="n">
         <v>0.11173125618255</v>
       </c>
-      <c r="AS4" s="0" t="n">
+      <c r="AS4" s="1" t="n">
         <v>0.08683612900858</v>
       </c>
-      <c r="AT4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="AV4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AW4" s="0" t="n">
+      <c r="AT4" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AV4" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW4" s="1" t="n">
         <v>0.334124998294213</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="n">
+      <c r="A5" s="1" t="n">
         <v>521</v>
       </c>
-      <c r="B5" s="0" t="s">
-        <v>59</v>
-      </c>
-      <c r="C5" s="2" t="n">
+      <c r="B5" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C5" s="3" t="n">
         <v>103075046108.167</v>
       </c>
-      <c r="D5" s="2" t="n">
+      <c r="D5" s="3" t="n">
         <v>103075046108.167</v>
       </c>
-      <c r="E5" s="2" t="n">
+      <c r="E5" s="3" t="n">
         <v>103075046108.167</v>
       </c>
-      <c r="F5" s="2" t="n">
+      <c r="F5" s="3" t="n">
         <v>103075046108.167</v>
       </c>
-      <c r="G5" s="2" t="n">
+      <c r="G5" s="3" t="n">
         <v>103075046108.167</v>
       </c>
-      <c r="H5" s="2" t="n">
+      <c r="H5" s="3" t="n">
         <v>103075046108.167</v>
       </c>
-      <c r="I5" s="2" t="n">
+      <c r="I5" s="3" t="n">
         <v>103075046108.167</v>
       </c>
-      <c r="J5" s="2" t="n">
+      <c r="J5" s="3" t="n">
         <v>103075046108.167</v>
       </c>
-      <c r="K5" s="0" t="n">
+      <c r="K5" s="1" t="n">
         <v>0.695479099736986</v>
       </c>
-      <c r="L5" s="0" t="n">
+      <c r="L5" s="1" t="n">
         <v>0.695479099736986</v>
       </c>
-      <c r="M5" s="0" t="n">
+      <c r="M5" s="1" t="n">
         <v>0.695479099736986</v>
       </c>
-      <c r="N5" s="0" t="n">
+      <c r="N5" s="1" t="n">
         <v>0.695479099736986</v>
       </c>
-      <c r="P5" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q5" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="R5" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="S5" s="0" t="n">
+      <c r="P5" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="R5" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="S5" s="1" t="n">
         <v>5001</v>
       </c>
-      <c r="T5" s="0" t="s">
+      <c r="T5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="U5" s="2" t="n">
+      <c r="U5" s="3" t="n">
         <v>165.158445920228</v>
       </c>
-      <c r="V5" s="0" t="n">
+      <c r="V5" s="1" t="n">
         <v>0.253374049777098</v>
       </c>
-      <c r="W5" s="0" t="n">
+      <c r="W5" s="1" t="n">
         <v>13084263798.3008</v>
       </c>
-      <c r="X5" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y5" s="0" t="s">
-        <v>60</v>
-      </c>
-      <c r="Z5" s="0" t="s">
-        <v>60</v>
-      </c>
-      <c r="AA5" s="2" t="n">
+      <c r="X5" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y5" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="Z5" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AA5" s="3" t="n">
         <v>103075046108.167</v>
       </c>
-      <c r="AB5" s="2" t="n">
+      <c r="AB5" s="3" t="n">
         <v>103075046108.167</v>
       </c>
-      <c r="AC5" s="0" t="n">
+      <c r="AC5" s="1" t="n">
         <v>0.695479099736986</v>
       </c>
-      <c r="AD5" s="0" t="n">
+      <c r="AD5" s="1" t="n">
         <v>0.695479099736986</v>
       </c>
-      <c r="AE5" s="0" t="n">
+      <c r="AE5" s="1" t="n">
         <v>0.695479099736986</v>
       </c>
-      <c r="AF5" s="0" t="n">
+      <c r="AF5" s="1" t="n">
         <v>0.695479099736986</v>
       </c>
-      <c r="AG5" s="0" t="n">
+      <c r="AG5" s="1" t="n">
         <v>0.439669166047023</v>
       </c>
-      <c r="AH5" s="0" t="n">
+      <c r="AH5" s="1" t="n">
         <v>0.439669166047023</v>
       </c>
-      <c r="AI5" s="0" t="n">
+      <c r="AI5" s="1" t="n">
         <v>0.448781890104464</v>
       </c>
-      <c r="AJ5" s="0" t="n">
+      <c r="AJ5" s="1" t="n">
         <v>0.448781890104464</v>
       </c>
-      <c r="AK5" s="0" t="n">
+      <c r="AK5" s="1" t="n">
         <v>0.448781890104464</v>
       </c>
-      <c r="AL5" s="0" t="n">
+      <c r="AL5" s="1" t="n">
         <v>0.448781890104464</v>
       </c>
-      <c r="AO5" s="0" t="s">
+      <c r="AO5" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="AQ5" s="0" t="n">
+      <c r="AQ5" s="1" t="n">
         <v>0.208561542801664</v>
       </c>
-      <c r="AR5" s="0" t="n">
+      <c r="AR5" s="1" t="n">
         <v>0.121463517867326</v>
       </c>
-      <c r="AS5" s="0" t="n">
+      <c r="AS5" s="1" t="n">
         <v>0.0952440285162229</v>
       </c>
-      <c r="AT5" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="AV5" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AW5" s="0" t="n">
+      <c r="AT5" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AV5" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW5" s="1" t="n">
         <v>0.362938802122111</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="n">
+      <c r="A6" s="1" t="n">
         <v>522</v>
       </c>
-      <c r="B6" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="C6" s="2" t="n">
+      <c r="B6" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C6" s="3" t="n">
         <v>108984647726.686</v>
       </c>
-      <c r="D6" s="2" t="n">
+      <c r="D6" s="3" t="n">
         <v>108984647726.686</v>
       </c>
-      <c r="E6" s="2" t="n">
+      <c r="E6" s="3" t="n">
         <v>108984647726.686</v>
       </c>
-      <c r="F6" s="2" t="n">
+      <c r="F6" s="3" t="n">
         <v>108984647726.686</v>
       </c>
-      <c r="G6" s="2" t="n">
+      <c r="G6" s="3" t="n">
         <v>108984647726.686</v>
       </c>
-      <c r="H6" s="2" t="n">
+      <c r="H6" s="3" t="n">
         <v>108984647726.686</v>
       </c>
-      <c r="I6" s="2" t="n">
+      <c r="I6" s="3" t="n">
         <v>108984647726.686</v>
       </c>
-      <c r="J6" s="2" t="n">
+      <c r="J6" s="3" t="n">
         <v>108984647726.686</v>
       </c>
-      <c r="K6" s="0" t="n">
+      <c r="K6" s="1" t="n">
         <v>0.721199307803459</v>
       </c>
-      <c r="L6" s="0" t="n">
+      <c r="L6" s="1" t="n">
         <v>0.721199307803459</v>
       </c>
-      <c r="M6" s="0" t="n">
+      <c r="M6" s="1" t="n">
         <v>0.721199307803459</v>
       </c>
-      <c r="N6" s="0" t="n">
+      <c r="N6" s="1" t="n">
         <v>0.721199307803459</v>
       </c>
-      <c r="P6" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q6" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="R6" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="S6" s="0" t="n">
+      <c r="P6" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="R6" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="S6" s="1" t="n">
         <v>5001</v>
       </c>
-      <c r="T6" s="0" t="s">
+      <c r="T6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="U6" s="2" t="n">
+      <c r="U6" s="3" t="n">
         <v>189.98450197224</v>
       </c>
-      <c r="V6" s="0" t="n">
+      <c r="V6" s="1" t="n">
         <v>0.285291578827518</v>
       </c>
-      <c r="W6" s="0" t="n">
+      <c r="W6" s="1" t="n">
         <v>16583918378.5642</v>
       </c>
-      <c r="X6" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y6" s="0" t="s">
-        <v>62</v>
-      </c>
-      <c r="Z6" s="0" t="s">
-        <v>62</v>
-      </c>
-      <c r="AA6" s="2" t="n">
+      <c r="X6" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y6" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="Z6" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="AA6" s="3" t="n">
         <v>108984647726.686</v>
       </c>
-      <c r="AB6" s="2" t="n">
+      <c r="AB6" s="3" t="n">
         <v>108984647726.686</v>
       </c>
-      <c r="AC6" s="0" t="n">
+      <c r="AC6" s="1" t="n">
         <v>0.721199307803459</v>
       </c>
-      <c r="AD6" s="0" t="n">
+      <c r="AD6" s="1" t="n">
         <v>0.721199307803459</v>
       </c>
-      <c r="AE6" s="0" t="n">
+      <c r="AE6" s="1" t="n">
         <v>0.721199307803459</v>
       </c>
-      <c r="AF6" s="0" t="n">
+      <c r="AF6" s="1" t="n">
         <v>0.721199307803459</v>
       </c>
-      <c r="AG6" s="0" t="n">
+      <c r="AG6" s="1" t="n">
         <v>0.468512536132473</v>
       </c>
-      <c r="AH6" s="0" t="n">
+      <c r="AH6" s="1" t="n">
         <v>0.468512536132473</v>
       </c>
-      <c r="AI6" s="0" t="n">
+      <c r="AI6" s="1" t="n">
         <v>0.477243036207156</v>
       </c>
-      <c r="AJ6" s="0" t="n">
+      <c r="AJ6" s="1" t="n">
         <v>0.477243036207156</v>
       </c>
-      <c r="AK6" s="0" t="n">
+      <c r="AK6" s="1" t="n">
         <v>0.477243036207156</v>
       </c>
-      <c r="AL6" s="0" t="n">
+      <c r="AL6" s="1" t="n">
         <v>0.477243036207156</v>
       </c>
-      <c r="AM6" s="0" t="s">
-        <v>63</v>
-      </c>
-      <c r="AN6" s="0" t="n">
+      <c r="AM6" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="AN6" s="1" t="n">
         <v>0.04</v>
       </c>
-      <c r="AO6" s="0" t="s">
+      <c r="AO6" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="AQ6" s="0" t="n">
+      <c r="AQ6" s="1" t="n">
         <v>0.232940405820522</v>
       </c>
-      <c r="AR6" s="0" t="n">
+      <c r="AR6" s="1" t="n">
         <v>0.132043500420345</v>
       </c>
-      <c r="AS6" s="0" t="n">
+      <c r="AS6" s="1" t="n">
         <v>0.104466022052903</v>
       </c>
-      <c r="AT6" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="AV6" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AW6" s="0" t="n">
+      <c r="AT6" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AV6" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW6" s="1" t="n">
         <v>0.394237410425195</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="n">
+      <c r="A7" s="1" t="n">
         <v>523</v>
       </c>
-      <c r="B7" s="0" t="s">
-        <v>64</v>
-      </c>
-      <c r="C7" s="2" t="n">
+      <c r="B7" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C7" s="3" t="n">
         <v>115233064534.8</v>
       </c>
-      <c r="D7" s="2" t="n">
+      <c r="D7" s="3" t="n">
         <v>115233064534.8</v>
       </c>
-      <c r="E7" s="2" t="n">
+      <c r="E7" s="3" t="n">
         <v>115233064534.8</v>
       </c>
-      <c r="F7" s="2" t="n">
+      <c r="F7" s="3" t="n">
         <v>115233064534.8</v>
       </c>
-      <c r="G7" s="2" t="n">
+      <c r="G7" s="3" t="n">
         <v>115233064534.8</v>
       </c>
-      <c r="H7" s="2" t="n">
+      <c r="H7" s="3" t="n">
         <v>115233064534.8</v>
       </c>
-      <c r="I7" s="2" t="n">
+      <c r="I7" s="3" t="n">
         <v>115233064534.8</v>
       </c>
-      <c r="J7" s="2" t="n">
+      <c r="J7" s="3" t="n">
         <v>115233064534.8</v>
       </c>
-      <c r="K7" s="0" t="n">
+      <c r="K7" s="1" t="n">
         <v>0.747870700604646</v>
       </c>
-      <c r="L7" s="0" t="n">
+      <c r="L7" s="1" t="n">
         <v>0.747870700604646</v>
       </c>
-      <c r="M7" s="0" t="n">
+      <c r="M7" s="1" t="n">
         <v>0.747870700604646</v>
       </c>
-      <c r="N7" s="0" t="n">
+      <c r="N7" s="1" t="n">
         <v>0.747870700604646</v>
       </c>
-      <c r="P7" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q7" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="R7" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="S7" s="0" t="n">
+      <c r="P7" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="R7" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="S7" s="1" t="n">
         <v>5001</v>
       </c>
-      <c r="T7" s="0" t="s">
+      <c r="T7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="U7" s="2" t="n">
+      <c r="U7" s="3" t="n">
         <v>218.542326361401</v>
       </c>
-      <c r="V7" s="0" t="n">
+      <c r="V7" s="1" t="n">
         <v>0.321229759012421</v>
       </c>
-      <c r="W7" s="0" t="n">
+      <c r="W7" s="1" t="n">
         <v>21019627319.238</v>
       </c>
-      <c r="X7" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y7" s="0" t="s">
-        <v>65</v>
-      </c>
-      <c r="Z7" s="0" t="s">
-        <v>65</v>
-      </c>
-      <c r="AA7" s="2" t="n">
+      <c r="X7" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y7" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="Z7" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="AA7" s="3" t="n">
         <v>115233064534.8</v>
       </c>
-      <c r="AB7" s="2" t="n">
+      <c r="AB7" s="3" t="n">
         <v>115233064534.8</v>
       </c>
-      <c r="AC7" s="0" t="n">
+      <c r="AC7" s="1" t="n">
         <v>0.747870700604646</v>
       </c>
-      <c r="AD7" s="0" t="n">
+      <c r="AD7" s="1" t="n">
         <v>0.747870700604646</v>
       </c>
-      <c r="AE7" s="0" t="n">
+      <c r="AE7" s="1" t="n">
         <v>0.747870700604646</v>
       </c>
-      <c r="AF7" s="0" t="n">
+      <c r="AF7" s="1" t="n">
         <v>0.747870700604646</v>
       </c>
-      <c r="AG7" s="0" t="n">
+      <c r="AG7" s="1" t="n">
         <v>0.499248101673351</v>
       </c>
-      <c r="AH7" s="0" t="n">
+      <c r="AH7" s="1" t="n">
         <v>0.499248101673351</v>
       </c>
-      <c r="AI7" s="0" t="n">
+      <c r="AI7" s="1" t="n">
         <v>0.507509150057746</v>
       </c>
-      <c r="AJ7" s="0" t="n">
+      <c r="AJ7" s="1" t="n">
         <v>0.507509150057746</v>
       </c>
-      <c r="AK7" s="0" t="n">
+      <c r="AK7" s="1" t="n">
         <v>0.507509150057746</v>
       </c>
-      <c r="AL7" s="0" t="n">
+      <c r="AL7" s="1" t="n">
         <v>0.507509150057746</v>
       </c>
-      <c r="AO7" s="0" t="s">
+      <c r="AO7" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="AQ7" s="0" t="n">
+      <c r="AQ7" s="1" t="n">
         <v>0.260168926327086</v>
       </c>
-      <c r="AR7" s="0" t="n">
+      <c r="AR7" s="1" t="n">
         <v>0.143545043889659</v>
       </c>
-      <c r="AS7" s="0" t="n">
+      <c r="AS7" s="1" t="n">
         <v>0.114580934191573</v>
       </c>
-      <c r="AT7" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="AV7" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AW7" s="0" t="n">
+      <c r="AT7" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AV7" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW7" s="1" t="n">
         <v>0.428235104293068</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="n">
+      <c r="A8" s="1" t="n">
         <v>524</v>
       </c>
-      <c r="B8" s="0" t="s">
-        <v>66</v>
-      </c>
-      <c r="C8" s="2" t="n">
+      <c r="B8" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C8" s="3" t="n">
         <v>121839721823.774</v>
       </c>
-      <c r="D8" s="2" t="n">
+      <c r="D8" s="3" t="n">
         <v>121839721823.774</v>
       </c>
-      <c r="E8" s="2" t="n">
+      <c r="E8" s="3" t="n">
         <v>121839721823.774</v>
       </c>
-      <c r="F8" s="2" t="n">
+      <c r="F8" s="3" t="n">
         <v>121839721823.774</v>
       </c>
-      <c r="G8" s="2" t="n">
+      <c r="G8" s="3" t="n">
         <v>121839721823.774</v>
       </c>
-      <c r="H8" s="2" t="n">
+      <c r="H8" s="3" t="n">
         <v>121839721823.774</v>
       </c>
-      <c r="I8" s="2" t="n">
+      <c r="I8" s="3" t="n">
         <v>121839721823.774</v>
       </c>
-      <c r="J8" s="2" t="n">
+      <c r="J8" s="3" t="n">
         <v>121839721823.774</v>
       </c>
-      <c r="K8" s="0" t="n">
+      <c r="K8" s="1" t="n">
         <v>0.775528454854407</v>
       </c>
-      <c r="L8" s="0" t="n">
+      <c r="L8" s="1" t="n">
         <v>0.775528454854407</v>
       </c>
-      <c r="M8" s="0" t="n">
+      <c r="M8" s="1" t="n">
         <v>0.775528454854407</v>
       </c>
-      <c r="N8" s="0" t="n">
+      <c r="N8" s="1" t="n">
         <v>0.775528454854407</v>
       </c>
-      <c r="P8" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q8" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="R8" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="S8" s="0" t="n">
+      <c r="P8" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="R8" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="S8" s="1" t="n">
         <v>5001</v>
       </c>
-      <c r="T8" s="0" t="s">
+      <c r="T8" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="U8" s="2" t="n">
+      <c r="U8" s="3" t="n">
         <v>251.392865816137</v>
       </c>
-      <c r="V8" s="0" t="n">
+      <c r="V8" s="1" t="n">
         <v>0.361695071755216</v>
       </c>
-      <c r="W8" s="0" t="n">
+      <c r="W8" s="1" t="n">
         <v>26641757548.1282</v>
       </c>
-      <c r="X8" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y8" s="0" t="s">
-        <v>67</v>
-      </c>
-      <c r="Z8" s="0" t="s">
-        <v>67</v>
-      </c>
-      <c r="AA8" s="2" t="n">
+      <c r="X8" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y8" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z8" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AA8" s="3" t="n">
         <v>121839721823.774</v>
       </c>
-      <c r="AB8" s="2" t="n">
+      <c r="AB8" s="3" t="n">
         <v>121839721823.774</v>
       </c>
-      <c r="AC8" s="0" t="n">
+      <c r="AC8" s="1" t="n">
         <v>0.775528454854407</v>
       </c>
-      <c r="AD8" s="0" t="n">
+      <c r="AD8" s="1" t="n">
         <v>0.775528454854407</v>
       </c>
-      <c r="AE8" s="0" t="n">
+      <c r="AE8" s="1" t="n">
         <v>0.775528454854407</v>
       </c>
-      <c r="AF8" s="0" t="n">
+      <c r="AF8" s="1" t="n">
         <v>0.775528454854407</v>
       </c>
-      <c r="AG8" s="0" t="n">
+      <c r="AG8" s="1" t="n">
         <v>0.531999995308491</v>
       </c>
-      <c r="AH8" s="0" t="n">
+      <c r="AH8" s="1" t="n">
         <v>0.531999995308491</v>
       </c>
-      <c r="AI8" s="0" t="n">
+      <c r="AI8" s="1" t="n">
         <v>0.539694700292147</v>
       </c>
-      <c r="AJ8" s="0" t="n">
+      <c r="AJ8" s="1" t="n">
         <v>0.539694700292147</v>
       </c>
-      <c r="AK8" s="0" t="n">
+      <c r="AK8" s="1" t="n">
         <v>0.539694700292147</v>
       </c>
-      <c r="AL8" s="0" t="n">
+      <c r="AL8" s="1" t="n">
         <v>0.539694700292147</v>
       </c>
-      <c r="AM8" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="AN8" s="0" t="n">
+      <c r="AM8" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="AN8" s="1" t="n">
         <v>0.09</v>
       </c>
-      <c r="AO8" s="0" t="s">
+      <c r="AO8" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="AQ8" s="0" t="n">
+      <c r="AQ8" s="1" t="n">
         <v>0.290580202209922</v>
       </c>
-      <c r="AR8" s="0" t="n">
+      <c r="AR8" s="1" t="n">
         <v>0.156048420101633</v>
       </c>
-      <c r="AS8" s="0" t="n">
+      <c r="AS8" s="1" t="n">
         <v>0.125675221686579</v>
       </c>
-      <c r="AT8" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="AV8" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AW8" s="0" t="n">
+      <c r="AT8" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AV8" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW8" s="1" t="n">
         <v>0.465164643687948</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="n">
+      <c r="A9" s="1" t="n">
         <v>518</v>
       </c>
-      <c r="B9" s="0" t="s">
-        <v>69</v>
-      </c>
-      <c r="C9" s="2" t="n">
+      <c r="B9" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C9" s="3" t="n">
         <v>128825158595.096</v>
       </c>
-      <c r="D9" s="2" t="n">
+      <c r="D9" s="3" t="n">
         <v>128825158595.096</v>
       </c>
-      <c r="E9" s="2" t="n">
+      <c r="E9" s="3" t="n">
         <v>128825158595.096</v>
       </c>
-      <c r="F9" s="2" t="n">
+      <c r="F9" s="3" t="n">
         <v>128825158595.096</v>
       </c>
-      <c r="G9" s="2" t="n">
+      <c r="G9" s="3" t="n">
         <v>128825158595.096</v>
       </c>
-      <c r="H9" s="2" t="n">
+      <c r="H9" s="3" t="n">
         <v>128825158595.096</v>
       </c>
-      <c r="I9" s="2" t="n">
+      <c r="I9" s="3" t="n">
         <v>128825158595.096</v>
       </c>
-      <c r="J9" s="2" t="n">
+      <c r="J9" s="3" t="n">
         <v>128825158595.096</v>
       </c>
-      <c r="K9" s="0" t="n">
+      <c r="K9" s="1" t="n">
         <v>0.804209048171833</v>
       </c>
-      <c r="L9" s="0" t="n">
+      <c r="L9" s="1" t="n">
         <v>0.804209048171833</v>
       </c>
-      <c r="M9" s="0" t="n">
+      <c r="M9" s="1" t="n">
         <v>0.804209048171833</v>
       </c>
-      <c r="N9" s="0" t="n">
+      <c r="N9" s="1" t="n">
         <v>0.804209048171833</v>
       </c>
-      <c r="P9" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q9" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="R9" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="S9" s="0" t="n">
+      <c r="P9" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="R9" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="S9" s="1" t="n">
         <v>5001</v>
       </c>
-      <c r="T9" s="0" t="s">
+      <c r="T9" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="U9" s="2" t="n">
+      <c r="U9" s="3" t="n">
         <v>289.181386669875</v>
       </c>
-      <c r="V9" s="0" t="n">
+      <c r="V9" s="1" t="n">
         <v>0.40725779994422</v>
       </c>
-      <c r="W9" s="0" t="n">
+      <c r="W9" s="1" t="n">
         <v>33767641760.4048</v>
       </c>
-      <c r="X9" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y9" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="Z9" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="AA9" s="2" t="n">
+      <c r="X9" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y9" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="Z9" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AA9" s="3" t="n">
         <v>128825158595.096</v>
       </c>
-      <c r="AB9" s="2" t="n">
+      <c r="AB9" s="3" t="n">
         <v>128825158595.096</v>
       </c>
-      <c r="AC9" s="0" t="n">
+      <c r="AC9" s="1" t="n">
         <v>0.804209048171833</v>
       </c>
-      <c r="AD9" s="0" t="n">
+      <c r="AD9" s="1" t="n">
         <v>0.804209048171833</v>
       </c>
-      <c r="AE9" s="0" t="n">
+      <c r="AE9" s="1" t="n">
         <v>0.804209048171833</v>
       </c>
-      <c r="AF9" s="0" t="n">
+      <c r="AF9" s="1" t="n">
         <v>0.804209048171833</v>
       </c>
-      <c r="AG9" s="0" t="n">
+      <c r="AG9" s="1" t="n">
         <v>0.566900493080717</v>
       </c>
-      <c r="AH9" s="0" t="n">
+      <c r="AH9" s="1" t="n">
         <v>0.566900493080717</v>
       </c>
-      <c r="AI9" s="0" t="n">
+      <c r="AI9" s="1" t="n">
         <v>0.573921414993776</v>
       </c>
-      <c r="AJ9" s="0" t="n">
+      <c r="AJ9" s="1" t="n">
         <v>0.573921414993776</v>
       </c>
-      <c r="AK9" s="0" t="n">
+      <c r="AK9" s="1" t="n">
         <v>0.573921414993776</v>
       </c>
-      <c r="AL9" s="0" t="n">
+      <c r="AL9" s="1" t="n">
         <v>0.573921414993776</v>
       </c>
-      <c r="AN9" s="0" t="n">
+      <c r="AN9" s="1" t="n">
         <v>0.05</v>
       </c>
-      <c r="AO9" s="0" t="s">
+      <c r="AO9" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="AQ9" s="0" t="n">
+      <c r="AQ9" s="1" t="n">
         <v>0.324546267336341</v>
       </c>
-      <c r="AR9" s="0" t="n">
+      <c r="AR9" s="1" t="n">
         <v>0.169640892895849</v>
       </c>
-      <c r="AS9" s="0" t="n">
+      <c r="AS9" s="1" t="n">
         <v>0.13784371245886</v>
       </c>
-      <c r="AT9" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="AV9" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AW9" s="0" t="n">
+      <c r="AT9" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AV9" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW9" s="1" t="n">
         <v>0.505278860999808</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="n">
+      <c r="A10" s="1" t="n">
         <v>519</v>
       </c>
-      <c r="B10" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="C10" s="2" t="n">
+      <c r="B10" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C10" s="3" t="n">
         <v>136211091412.829</v>
       </c>
-      <c r="D10" s="2" t="n">
+      <c r="D10" s="3" t="n">
         <v>136211091412.829</v>
       </c>
-      <c r="E10" s="2" t="n">
+      <c r="E10" s="3" t="n">
         <v>136211091412.829</v>
       </c>
-      <c r="F10" s="2" t="n">
+      <c r="F10" s="3" t="n">
         <v>136211091412.829</v>
       </c>
-      <c r="G10" s="2" t="n">
+      <c r="G10" s="3" t="n">
         <v>136211091412.829</v>
       </c>
-      <c r="H10" s="2" t="n">
+      <c r="H10" s="3" t="n">
         <v>136211091412.829</v>
       </c>
-      <c r="I10" s="2" t="n">
+      <c r="I10" s="3" t="n">
         <v>136211091412.829</v>
       </c>
-      <c r="J10" s="2" t="n">
+      <c r="J10" s="3" t="n">
         <v>136211091412.829</v>
       </c>
-      <c r="K10" s="0" t="n">
+      <c r="K10" s="1" t="n">
         <v>0.833950307191324</v>
       </c>
-      <c r="L10" s="0" t="n">
+      <c r="L10" s="1" t="n">
         <v>0.833950307191324</v>
       </c>
-      <c r="M10" s="0" t="n">
+      <c r="M10" s="1" t="n">
         <v>0.833950307191324</v>
       </c>
-      <c r="N10" s="0" t="n">
+      <c r="N10" s="1" t="n">
         <v>0.833950307191324</v>
       </c>
-      <c r="P10" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q10" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="R10" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="S10" s="0" t="n">
+      <c r="P10" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="R10" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="S10" s="1" t="n">
         <v>5001</v>
       </c>
-      <c r="T10" s="0" t="s">
+      <c r="T10" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="U10" s="2" t="n">
+      <c r="U10" s="3" t="n">
         <v>332.650149497376</v>
       </c>
-      <c r="V10" s="0" t="n">
+      <c r="V10" s="1" t="n">
         <v>0.458560065003193</v>
       </c>
-      <c r="W10" s="0" t="n">
+      <c r="W10" s="1" t="n">
         <v>42799489785.8812</v>
       </c>
-      <c r="X10" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y10" s="0" t="s">
-        <v>72</v>
-      </c>
-      <c r="Z10" s="0" t="s">
-        <v>72</v>
-      </c>
-      <c r="AA10" s="2" t="n">
+      <c r="X10" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y10" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="Z10" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="AA10" s="3" t="n">
         <v>136211091412.829</v>
       </c>
-      <c r="AB10" s="2" t="n">
+      <c r="AB10" s="3" t="n">
         <v>136211091412.829</v>
       </c>
-      <c r="AC10" s="0" t="n">
+      <c r="AC10" s="1" t="n">
         <v>0.833950307191324</v>
       </c>
-      <c r="AD10" s="0" t="n">
+      <c r="AD10" s="1" t="n">
         <v>0.833950307191324</v>
       </c>
-      <c r="AE10" s="0" t="n">
+      <c r="AE10" s="1" t="n">
         <v>0.833950307191324</v>
       </c>
-      <c r="AF10" s="0" t="n">
+      <c r="AF10" s="1" t="n">
         <v>0.833950307191324</v>
       </c>
-      <c r="AG10" s="0" t="n">
+      <c r="AG10" s="1" t="n">
         <v>0.604090548664015</v>
       </c>
-      <c r="AH10" s="0" t="n">
+      <c r="AH10" s="1" t="n">
         <v>0.604090548664015</v>
       </c>
-      <c r="AI10" s="0" t="n">
+      <c r="AI10" s="1" t="n">
         <v>0.610318742077986</v>
       </c>
-      <c r="AJ10" s="0" t="n">
+      <c r="AJ10" s="1" t="n">
         <v>0.610318742077986</v>
       </c>
-      <c r="AK10" s="0" t="n">
+      <c r="AK10" s="1" t="n">
         <v>0.610318742077986</v>
       </c>
-      <c r="AL10" s="0" t="n">
+      <c r="AL10" s="1" t="n">
         <v>0.610318742077986</v>
       </c>
-      <c r="AO10" s="0" t="s">
+      <c r="AO10" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="AQ10" s="0" t="n">
+      <c r="AQ10" s="1" t="n">
         <v>0.362482642798419</v>
       </c>
-      <c r="AR10" s="0" t="n">
+      <c r="AR10" s="1" t="n">
         <v>0.184417327158828</v>
       </c>
-      <c r="AS10" s="0" t="n">
+      <c r="AS10" s="1" t="n">
         <v>0.151190416133318</v>
       </c>
-      <c r="AT10" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="AV10" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AW10" s="0" t="n">
+      <c r="AT10" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AV10" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW10" s="1" t="n">
         <v>0.548852392024304</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="n">
+      <c r="A11" s="1" t="n">
         <v>520</v>
       </c>
-      <c r="B11" s="0" t="s">
-        <v>73</v>
-      </c>
-      <c r="C11" s="2" t="n">
+      <c r="B11" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C11" s="3" t="n">
         <v>144020481916.801</v>
       </c>
-      <c r="D11" s="2" t="n">
+      <c r="D11" s="3" t="n">
         <v>144020481916.801</v>
       </c>
-      <c r="E11" s="2" t="n">
+      <c r="E11" s="3" t="n">
         <v>144020481916.801</v>
       </c>
-      <c r="F11" s="2" t="n">
+      <c r="F11" s="3" t="n">
         <v>144020481916.801</v>
       </c>
-      <c r="G11" s="2" t="n">
+      <c r="G11" s="3" t="n">
         <v>144020481916.801</v>
       </c>
-      <c r="H11" s="2" t="n">
+      <c r="H11" s="3" t="n">
         <v>144020481916.801</v>
       </c>
-      <c r="I11" s="2" t="n">
+      <c r="I11" s="3" t="n">
         <v>144020481916.801</v>
       </c>
-      <c r="J11" s="2" t="n">
+      <c r="J11" s="3" t="n">
         <v>144020481916.801</v>
       </c>
-      <c r="K11" s="0" t="n">
+      <c r="K11" s="1" t="n">
         <v>0.864791457451874</v>
       </c>
-      <c r="L11" s="0" t="n">
+      <c r="L11" s="1" t="n">
         <v>0.864791457451874</v>
       </c>
-      <c r="M11" s="0" t="n">
+      <c r="M11" s="1" t="n">
         <v>0.864791457451874</v>
       </c>
-      <c r="N11" s="0" t="n">
+      <c r="N11" s="1" t="n">
         <v>0.864791457451874</v>
       </c>
-      <c r="P11" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q11" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="R11" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="S11" s="0" t="n">
+      <c r="P11" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q11" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="R11" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="S11" s="1" t="n">
         <v>5001</v>
       </c>
-      <c r="T11" s="0" t="s">
+      <c r="T11" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="U11" s="2" t="n">
+      <c r="U11" s="3" t="n">
         <v>382.652988959313</v>
       </c>
-      <c r="V11" s="0" t="n">
+      <c r="V11" s="1" t="n">
         <v>0.516324876391646</v>
       </c>
-      <c r="W11" s="0" t="n">
+      <c r="W11" s="1" t="n">
         <v>54247090718.6557</v>
       </c>
-      <c r="X11" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y11" s="0" t="s">
-        <v>74</v>
-      </c>
-      <c r="Z11" s="0" t="s">
-        <v>74</v>
-      </c>
-      <c r="AA11" s="2" t="n">
+      <c r="X11" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y11" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="Z11" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="AA11" s="3" t="n">
         <v>144020481916.801</v>
       </c>
-      <c r="AB11" s="2" t="n">
+      <c r="AB11" s="3" t="n">
         <v>144020481916.801</v>
       </c>
-      <c r="AC11" s="0" t="n">
+      <c r="AC11" s="1" t="n">
         <v>0.864791457451874</v>
       </c>
-      <c r="AD11" s="0" t="n">
+      <c r="AD11" s="1" t="n">
         <v>0.864791457451874</v>
       </c>
-      <c r="AE11" s="0" t="n">
+      <c r="AE11" s="1" t="n">
         <v>0.864791457451874</v>
       </c>
-      <c r="AF11" s="0" t="n">
+      <c r="AF11" s="1" t="n">
         <v>0.864791457451874</v>
       </c>
-      <c r="AG11" s="0" t="n">
+      <c r="AG11" s="1" t="n">
         <v>0.643720362637313</v>
       </c>
-      <c r="AH11" s="0" t="n">
+      <c r="AH11" s="1" t="n">
         <v>0.643720362637313</v>
       </c>
-      <c r="AI11" s="0" t="n">
+      <c r="AI11" s="1" t="n">
         <v>0.649024338873457</v>
       </c>
-      <c r="AJ11" s="0" t="n">
+      <c r="AJ11" s="1" t="n">
         <v>0.649024338873457</v>
       </c>
-      <c r="AK11" s="0" t="n">
+      <c r="AK11" s="1" t="n">
         <v>0.649024338873457</v>
       </c>
-      <c r="AL11" s="0" t="n">
+      <c r="AL11" s="1" t="n">
         <v>0.649024338873457</v>
       </c>
-      <c r="AN11" s="0" t="n">
+      <c r="AN11" s="1" t="n">
         <v>0.07</v>
       </c>
-      <c r="AO11" s="0" t="s">
+      <c r="AO11" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="AQ11" s="0" t="n">
+      <c r="AQ11" s="1" t="n">
         <v>0.404853420156448</v>
       </c>
-      <c r="AR11" s="0" t="n">
+      <c r="AR11" s="1" t="n">
         <v>0.200480850907136</v>
       </c>
-      <c r="AS11" s="0" t="n">
+      <c r="AS11" s="1" t="n">
         <v>0.165829413056385</v>
       </c>
-      <c r="AT11" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="AV11" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AW11" s="0" t="n">
+      <c r="AT11" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AV11" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW11" s="1" t="n">
         <v>0.596183556214347</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="n">
+      <c r="A12" s="1" t="n">
         <v>521</v>
       </c>
-      <c r="B12" s="0" t="s">
-        <v>75</v>
-      </c>
-      <c r="C12" s="2" t="n">
+      <c r="B12" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C12" s="3" t="n">
         <v>152277608206.537</v>
       </c>
-      <c r="D12" s="2" t="n">
+      <c r="D12" s="3" t="n">
         <v>152277608206.537</v>
       </c>
-      <c r="E12" s="2" t="n">
+      <c r="E12" s="3" t="n">
         <v>152277608206.537</v>
       </c>
-      <c r="F12" s="2" t="n">
+      <c r="F12" s="3" t="n">
         <v>152277608206.537</v>
       </c>
-      <c r="G12" s="2" t="n">
+      <c r="G12" s="3" t="n">
         <v>152277608206.537</v>
       </c>
-      <c r="H12" s="2" t="n">
+      <c r="H12" s="3" t="n">
         <v>152277608206.537</v>
       </c>
-      <c r="I12" s="2" t="n">
+      <c r="I12" s="3" t="n">
         <v>152277608206.537</v>
       </c>
-      <c r="J12" s="2" t="n">
+      <c r="J12" s="3" t="n">
         <v>152277608206.537</v>
       </c>
-      <c r="K12" s="0" t="n">
+      <c r="K12" s="1" t="n">
         <v>0.896773175131359</v>
       </c>
-      <c r="L12" s="0" t="n">
+      <c r="L12" s="1" t="n">
         <v>0.896773175131359</v>
       </c>
-      <c r="M12" s="0" t="n">
+      <c r="M12" s="1" t="n">
         <v>0.896773175131359</v>
       </c>
-      <c r="N12" s="0" t="n">
+      <c r="N12" s="1" t="n">
         <v>0.896773175131359</v>
       </c>
-      <c r="P12" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q12" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="R12" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="S12" s="0" t="n">
+      <c r="P12" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q12" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="R12" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="S12" s="1" t="n">
         <v>5001</v>
       </c>
-      <c r="T12" s="0" t="s">
+      <c r="T12" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="U12" s="2" t="n">
+      <c r="U12" s="3" t="n">
         <v>440.172085239515</v>
       </c>
-      <c r="V12" s="0" t="n">
+      <c r="V12" s="1" t="n">
         <v>0.581366321070701</v>
       </c>
-      <c r="W12" s="0" t="n">
+      <c r="W12" s="1" t="n">
         <v>68756587196.7199</v>
       </c>
-      <c r="X12" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y12" s="0" t="s">
-        <v>76</v>
-      </c>
-      <c r="Z12" s="0" t="s">
-        <v>76</v>
-      </c>
-      <c r="AA12" s="2" t="n">
+      <c r="X12" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y12" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="Z12" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="AA12" s="3" t="n">
         <v>152277608206.537</v>
       </c>
-      <c r="AB12" s="2" t="n">
+      <c r="AB12" s="3" t="n">
         <v>152277608206.537</v>
       </c>
-      <c r="AC12" s="0" t="n">
+      <c r="AC12" s="1" t="n">
         <v>0.896773175131359</v>
       </c>
-      <c r="AD12" s="0" t="n">
+      <c r="AD12" s="1" t="n">
         <v>0.896773175131359</v>
       </c>
-      <c r="AE12" s="0" t="n">
+      <c r="AE12" s="1" t="n">
         <v>0.896773175131359</v>
       </c>
-      <c r="AF12" s="0" t="n">
+      <c r="AF12" s="1" t="n">
         <v>0.896773175131359</v>
       </c>
-      <c r="AG12" s="0" t="n">
+      <c r="AG12" s="1" t="n">
         <v>0.685949989104005</v>
       </c>
-      <c r="AH12" s="0" t="n">
+      <c r="AH12" s="1" t="n">
         <v>0.685949989104005</v>
       </c>
-      <c r="AI12" s="0" t="n">
+      <c r="AI12" s="1" t="n">
         <v>0.690184592752198</v>
       </c>
-      <c r="AJ12" s="0" t="n">
+      <c r="AJ12" s="1" t="n">
         <v>0.690184592752198</v>
       </c>
-      <c r="AK12" s="0" t="n">
+      <c r="AK12" s="1" t="n">
         <v>0.690184592752198</v>
       </c>
-      <c r="AL12" s="0" t="n">
+      <c r="AL12" s="1" t="n">
         <v>0.690184592752198</v>
       </c>
-      <c r="AO12" s="0" t="s">
+      <c r="AO12" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="AQ12" s="0" t="n">
+      <c r="AQ12" s="1" t="n">
         <v>0.452176938865245</v>
       </c>
-      <c r="AR12" s="0" t="n">
+      <c r="AR12" s="1" t="n">
         <v>0.217943575040721</v>
       </c>
-      <c r="AS12" s="0" t="n">
+      <c r="AS12" s="1" t="n">
         <v>0.181885829392628</v>
       </c>
-      <c r="AT12" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="AV12" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AW12" s="0" t="n">
+      <c r="AT12" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AV12" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW12" s="1" t="n">
         <v>0.647596399078182</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="n">
+      <c r="A13" s="1" t="n">
         <v>522</v>
       </c>
-      <c r="B13" s="0" t="s">
-        <v>77</v>
-      </c>
-      <c r="C13" s="2" t="n">
+      <c r="B13" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C13" s="3" t="n">
         <v>161008140317.842</v>
       </c>
-      <c r="D13" s="2" t="n">
+      <c r="D13" s="3" t="n">
         <v>161008140317.842</v>
       </c>
-      <c r="E13" s="2" t="n">
+      <c r="E13" s="3" t="n">
         <v>161008140317.842</v>
       </c>
-      <c r="F13" s="2" t="n">
+      <c r="F13" s="3" t="n">
         <v>161008140317.842</v>
       </c>
-      <c r="G13" s="2" t="n">
+      <c r="G13" s="3" t="n">
         <v>161008140317.842</v>
       </c>
-      <c r="H13" s="2" t="n">
+      <c r="H13" s="3" t="n">
         <v>161008140317.842</v>
       </c>
-      <c r="I13" s="2" t="n">
+      <c r="I13" s="3" t="n">
         <v>161008140317.842</v>
       </c>
-      <c r="J13" s="2" t="n">
+      <c r="J13" s="3" t="n">
         <v>161008140317.842</v>
       </c>
-      <c r="K13" s="0" t="n">
+      <c r="K13" s="1" t="n">
         <v>0.929937640694067</v>
       </c>
-      <c r="L13" s="0" t="n">
+      <c r="L13" s="1" t="n">
         <v>0.929937640694067</v>
       </c>
-      <c r="M13" s="0" t="n">
+      <c r="M13" s="1" t="n">
         <v>0.929937640694067</v>
       </c>
-      <c r="N13" s="0" t="n">
+      <c r="N13" s="1" t="n">
         <v>0.929937640694067</v>
       </c>
-      <c r="P13" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q13" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="R13" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="S13" s="0" t="n">
+      <c r="P13" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q13" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="R13" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="S13" s="1" t="n">
         <v>5001</v>
       </c>
-      <c r="T13" s="0" t="s">
+      <c r="T13" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="U13" s="2" t="n">
+      <c r="U13" s="3" t="n">
         <v>506.337256507629</v>
       </c>
-      <c r="V13" s="0" t="n">
+      <c r="V13" s="1" t="n">
         <v>0.654601036535977</v>
       </c>
-      <c r="W13" s="0" t="n">
+      <c r="W13" s="1" t="n">
         <v>87146945952.5202</v>
       </c>
-      <c r="X13" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y13" s="0" t="s">
-        <v>78</v>
-      </c>
-      <c r="Z13" s="0" t="s">
-        <v>78</v>
-      </c>
-      <c r="AA13" s="2" t="n">
+      <c r="X13" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y13" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="Z13" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AA13" s="3" t="n">
         <v>161008140317.842</v>
       </c>
-      <c r="AB13" s="2" t="n">
+      <c r="AB13" s="3" t="n">
         <v>161008140317.842</v>
       </c>
-      <c r="AC13" s="0" t="n">
+      <c r="AC13" s="1" t="n">
         <v>0.929937640694067</v>
       </c>
-      <c r="AD13" s="0" t="n">
+      <c r="AD13" s="1" t="n">
         <v>0.929937640694067</v>
       </c>
-      <c r="AE13" s="0" t="n">
+      <c r="AE13" s="1" t="n">
         <v>0.929937640694067</v>
       </c>
-      <c r="AF13" s="0" t="n">
+      <c r="AF13" s="1" t="n">
         <v>0.929937640694067</v>
       </c>
-      <c r="AG13" s="0" t="n">
+      <c r="AG13" s="1" t="n">
         <v>0.730949982107201</v>
       </c>
-      <c r="AH13" s="0" t="n">
+      <c r="AH13" s="1" t="n">
         <v>0.730949982107201</v>
       </c>
-      <c r="AI13" s="0" t="n">
+      <c r="AI13" s="1" t="n">
         <v>0.733955174777188</v>
       </c>
-      <c r="AJ13" s="0" t="n">
+      <c r="AJ13" s="1" t="n">
         <v>0.733955174777188</v>
       </c>
-      <c r="AK13" s="0" t="n">
+      <c r="AK13" s="1" t="n">
         <v>0.733955174777188</v>
       </c>
-      <c r="AL13" s="0" t="n">
+      <c r="AL13" s="1" t="n">
         <v>0.733955174777188</v>
       </c>
-      <c r="AN13" s="0" t="n">
+      <c r="AN13" s="1" t="n">
         <v>0.04</v>
       </c>
-      <c r="AO13" s="0" t="s">
+      <c r="AO13" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="AQ13" s="0" t="n">
+      <c r="AQ13" s="1" t="n">
         <v>0.505032127337673</v>
       </c>
-      <c r="AR13" s="0" t="n">
+      <c r="AR13" s="1" t="n">
         <v>0.236927375789783</v>
       </c>
-      <c r="AS13" s="0" t="n">
+      <c r="AS13" s="1" t="n">
         <v>0.199496906634986</v>
       </c>
-      <c r="AT13" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="AV13" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AW13" s="0" t="n">
+      <c r="AT13" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AV13" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW13" s="1" t="n">
         <v>0.703442910706927</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="n">
+      <c r="A14" s="1" t="n">
         <v>523</v>
       </c>
-      <c r="B14" s="0" t="s">
-        <v>79</v>
-      </c>
-      <c r="C14" s="2" t="n">
+      <c r="B14" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C14" s="3" t="n">
         <v>170239220026.685</v>
       </c>
-      <c r="D14" s="2" t="n">
+      <c r="D14" s="3" t="n">
         <v>170239220026.685</v>
       </c>
-      <c r="E14" s="2" t="n">
+      <c r="E14" s="3" t="n">
         <v>170239220026.685</v>
       </c>
-      <c r="F14" s="2" t="n">
+      <c r="F14" s="3" t="n">
         <v>170239220026.685</v>
       </c>
-      <c r="G14" s="2" t="n">
+      <c r="G14" s="3" t="n">
         <v>170239220026.685</v>
       </c>
-      <c r="H14" s="2" t="n">
+      <c r="H14" s="3" t="n">
         <v>170239220026.685</v>
       </c>
-      <c r="I14" s="2" t="n">
+      <c r="I14" s="3" t="n">
         <v>170239220026.685</v>
       </c>
-      <c r="J14" s="2" t="n">
+      <c r="J14" s="3" t="n">
         <v>170239220026.685</v>
       </c>
-      <c r="K14" s="0" t="n">
+      <c r="K14" s="1" t="n">
         <v>0.964328594522215</v>
       </c>
-      <c r="L14" s="0" t="n">
+      <c r="L14" s="1" t="n">
         <v>0.964328594522215</v>
       </c>
-      <c r="M14" s="0" t="n">
+      <c r="M14" s="1" t="n">
         <v>0.964328594522215</v>
       </c>
-      <c r="N14" s="0" t="n">
+      <c r="N14" s="1" t="n">
         <v>0.964328594522215</v>
       </c>
-      <c r="P14" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q14" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="R14" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="S14" s="0" t="n">
+      <c r="P14" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q14" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="R14" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="S14" s="1" t="n">
         <v>5001</v>
       </c>
-      <c r="T14" s="0" t="s">
+      <c r="T14" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="U14" s="2" t="n">
+      <c r="U14" s="3" t="n">
         <v>582.448151359183</v>
       </c>
-      <c r="V14" s="0" t="n">
+      <c r="V14" s="1" t="n">
         <v>0.737061129108414</v>
       </c>
-      <c r="W14" s="0" t="n">
+      <c r="W14" s="1" t="n">
         <v>110456183159.914</v>
       </c>
-      <c r="X14" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y14" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="Z14" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="AA14" s="2" t="n">
+      <c r="X14" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y14" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="Z14" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="AA14" s="3" t="n">
         <v>170239220026.685</v>
       </c>
-      <c r="AB14" s="2" t="n">
+      <c r="AB14" s="3" t="n">
         <v>170239220026.685</v>
       </c>
-      <c r="AC14" s="0" t="n">
+      <c r="AC14" s="1" t="n">
         <v>0.964328594522215</v>
       </c>
-      <c r="AD14" s="0" t="n">
+      <c r="AD14" s="1" t="n">
         <v>0.964328594522215</v>
       </c>
-      <c r="AE14" s="0" t="n">
+      <c r="AE14" s="1" t="n">
         <v>0.964328594522215</v>
       </c>
-      <c r="AF14" s="0" t="n">
+      <c r="AF14" s="1" t="n">
         <v>0.964328594522215</v>
       </c>
-      <c r="AG14" s="0" t="n">
+      <c r="AG14" s="1" t="n">
         <v>0.77890208445139</v>
       </c>
-      <c r="AH14" s="0" t="n">
+      <c r="AH14" s="1" t="n">
         <v>0.77890208445139</v>
       </c>
-      <c r="AI14" s="0" t="n">
+      <c r="AI14" s="1" t="n">
         <v>0.780501628461623</v>
       </c>
-      <c r="AJ14" s="0" t="n">
+      <c r="AJ14" s="1" t="n">
         <v>0.780501628461623</v>
       </c>
-      <c r="AK14" s="0" t="n">
+      <c r="AK14" s="1" t="n">
         <v>0.780501628461623</v>
       </c>
-      <c r="AL14" s="0" t="n">
+      <c r="AL14" s="1" t="n">
         <v>0.780501628461623</v>
       </c>
-      <c r="AO14" s="0" t="s">
+      <c r="AO14" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="AQ14" s="0" t="n">
+      <c r="AQ14" s="1" t="n">
         <v>0.564065585218237</v>
       </c>
-      <c r="AR14" s="0" t="n">
+      <c r="AR14" s="1" t="n">
         <v>0.257564745316052</v>
       </c>
-      <c r="AS14" s="0" t="n">
+      <c r="AS14" s="1" t="n">
         <v>0.218813174670228</v>
       </c>
-      <c r="AT14" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="AV14" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AW14" s="0" t="n">
+      <c r="AT14" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AV14" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW14" s="1" t="n">
         <v>0.764105435620396</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="n">
+      <c r="A15" s="1" t="n">
         <v>524</v>
       </c>
-      <c r="B15" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="C15" s="2" t="n">
+      <c r="B15" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C15" s="3" t="n">
         <v>180000000000</v>
       </c>
-      <c r="D15" s="2" t="n">
+      <c r="D15" s="3" t="n">
         <v>180000000000</v>
       </c>
-      <c r="E15" s="2" t="n">
+      <c r="E15" s="3" t="n">
         <v>180000000000</v>
       </c>
-      <c r="F15" s="2" t="n">
+      <c r="F15" s="3" t="n">
         <v>180000000000</v>
       </c>
-      <c r="G15" s="2" t="n">
+      <c r="G15" s="3" t="n">
         <v>180000000000</v>
       </c>
-      <c r="H15" s="2" t="n">
+      <c r="H15" s="3" t="n">
         <v>180000000000</v>
       </c>
-      <c r="I15" s="2" t="n">
+      <c r="I15" s="3" t="n">
         <v>180000000000</v>
       </c>
-      <c r="J15" s="2" t="n">
+      <c r="J15" s="3" t="n">
         <v>180000000000</v>
       </c>
-      <c r="K15" s="0" t="n">
+      <c r="K15" s="1" t="n">
         <v>0.999991394604835</v>
       </c>
-      <c r="L15" s="0" t="n">
+      <c r="L15" s="1" t="n">
         <v>0.999991394604835</v>
       </c>
-      <c r="M15" s="0" t="n">
+      <c r="M15" s="1" t="n">
         <v>0.999991394604835</v>
       </c>
-      <c r="N15" s="0" t="n">
+      <c r="N15" s="1" t="n">
         <v>0.999991394604835</v>
       </c>
-      <c r="P15" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q15" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="R15" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="S15" s="0" t="n">
+      <c r="P15" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q15" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="R15" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="S15" s="1" t="n">
         <v>5001</v>
       </c>
-      <c r="T15" s="0" t="s">
+      <c r="T15" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="U15" s="2" t="n">
+      <c r="U15" s="3" t="n">
         <v>669.999777147781</v>
       </c>
-      <c r="V15" s="0" t="n">
+      <c r="V15" s="1" t="n">
         <v>0.829908719542201</v>
       </c>
-      <c r="W15" s="0" t="n">
+      <c r="W15" s="1" t="n">
         <v>139999953697.787</v>
       </c>
-      <c r="X15" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y15" s="0" t="s">
-        <v>82</v>
-      </c>
-      <c r="Z15" s="0" t="s">
-        <v>82</v>
-      </c>
-      <c r="AA15" s="2" t="n">
+      <c r="X15" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y15" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="Z15" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AA15" s="3" t="n">
         <v>180000000000</v>
       </c>
-      <c r="AB15" s="2" t="n">
+      <c r="AB15" s="3" t="n">
         <v>180000000000</v>
       </c>
-      <c r="AC15" s="0" t="n">
+      <c r="AC15" s="1" t="n">
         <v>0.999991394604835</v>
       </c>
-      <c r="AD15" s="0" t="n">
+      <c r="AD15" s="1" t="n">
         <v>0.999991394604835</v>
       </c>
-      <c r="AE15" s="0" t="n">
+      <c r="AE15" s="1" t="n">
         <v>0.999991394604835</v>
       </c>
-      <c r="AF15" s="0" t="n">
+      <c r="AF15" s="1" t="n">
         <v>0.999991394604835</v>
       </c>
-      <c r="AG15" s="0" t="n">
+      <c r="AG15" s="1" t="n">
         <v>0.829999961712487</v>
       </c>
-      <c r="AH15" s="0" t="n">
+      <c r="AH15" s="1" t="n">
         <v>0.829999961712487</v>
       </c>
-      <c r="AI15" s="0" t="n">
+      <c r="AI15" s="1" t="n">
         <v>0.829999995866477</v>
       </c>
-      <c r="AJ15" s="0" t="n">
+      <c r="AJ15" s="1" t="n">
         <v>0.829999995866477</v>
       </c>
-      <c r="AK15" s="0" t="n">
+      <c r="AK15" s="1" t="n">
         <v>0.829999995866477</v>
       </c>
-      <c r="AL15" s="0" t="n">
+      <c r="AL15" s="1" t="n">
         <v>0.829999995866477</v>
       </c>
-      <c r="AN15" s="0" t="n">
+      <c r="AN15" s="1" t="n">
         <v>0.09</v>
       </c>
-      <c r="AO15" s="0" t="s">
+      <c r="AO15" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="AQ15" s="0" t="n">
+      <c r="AQ15" s="1" t="n">
         <v>0.62999949350719</v>
       </c>
-      <c r="AR15" s="0" t="n">
+      <c r="AR15" s="1" t="n">
         <v>0.27999971640501</v>
       </c>
-      <c r="AS15" s="0" t="n">
+      <c r="AS15" s="1" t="n">
         <v>0.239999738426356</v>
       </c>
-      <c r="AT15" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="AV15" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AW15" s="0" t="n">
+      <c r="AT15" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AV15" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW15" s="1" t="n">
         <v>0.829999290429818</v>
       </c>
     </row>

</xml_diff>